<commit_message>
Completed the development procedure and made admin controls into it
</commit_message>
<xml_diff>
--- a/Attendance2022.xlsx
+++ b/Attendance2022.xlsx
@@ -604,7 +604,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anita24feb.sinha@gmail.com</t>
+          <t>avinash18dce.kumar@gmail.com</t>
         </is>
       </c>
     </row>
@@ -799,7 +799,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anita24feb.sinha@gmail.com</t>
+          <t>avinash18dce.kumar@gmail.com</t>
         </is>
       </c>
     </row>
@@ -989,7 +989,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anita24feb.sinha@gmail.com</t>
+          <t>avinash18dce.kumar@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anita24feb.sinha@gmail.com</t>
+          <t>avinash18dce.kumar@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1359,7 +1359,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anita24feb.sinha@gmail.com</t>
+          <t>avinash18dce.kumar@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1554,7 +1554,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anita24feb.sinha@gmail.com</t>
+          <t>avinash18dce.kumar@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1744,7 +1744,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anita24feb.sinha@gmail.com</t>
+          <t>avinash18dce.kumar@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1940,11 +1940,21 @@
           <t>P</t>
         </is>
       </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anita24feb.sinha@gmail.com</t>
+          <t>avinash18dce.kumar@gmail.com</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>P</t>
         </is>
       </c>
     </row>
@@ -2134,7 +2144,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anita24feb.sinha@gmail.com</t>
+          <t>avinash18dce.kumar@gmail.com</t>
         </is>
       </c>
     </row>
@@ -2329,7 +2339,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anita24feb.sinha@gmail.com</t>
+          <t>avinash18dce.kumar@gmail.com</t>
         </is>
       </c>
     </row>
@@ -2524,7 +2534,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anita24feb.sinha@gmail.com</t>
+          <t>avinash18dce.kumar@gmail.com</t>
         </is>
       </c>
     </row>
@@ -2714,7 +2724,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anita24feb.sinha@gmail.com</t>
+          <t>avinash18dce.kumar@gmail.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue regarding going back after giving attendance and then going forward to view solved
</commit_message>
<xml_diff>
--- a/Attendance2022.xlsx
+++ b/Attendance2022.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -605,6 +605,13 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>avinash18dce.kumar@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fakeid@gmail.com</t>
         </is>
       </c>
     </row>
@@ -619,7 +626,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -800,6 +807,13 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>avinash18dce.kumar@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fakeid@gmail.com</t>
         </is>
       </c>
     </row>
@@ -814,7 +828,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -990,6 +1004,13 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>avinash18dce.kumar@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fakeid@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1004,7 +1025,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1180,6 +1201,13 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>avinash18dce.kumar@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fakeid@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1222,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1360,6 +1388,13 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>avinash18dce.kumar@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fakeid@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1374,7 +1409,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1555,6 +1590,13 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>avinash18dce.kumar@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fakeid@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1611,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1745,6 +1787,13 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>avinash18dce.kumar@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fakeid@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1759,7 +1808,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1953,6 +2002,18 @@
         </is>
       </c>
       <c r="AB3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fakeid@gmail.com</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
         <is>
           <t>P</t>
         </is>
@@ -1969,7 +2030,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2145,6 +2206,13 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>avinash18dce.kumar@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fakeid@gmail.com</t>
         </is>
       </c>
     </row>
@@ -2159,7 +2227,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2340,6 +2408,13 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>avinash18dce.kumar@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fakeid@gmail.com</t>
         </is>
       </c>
     </row>
@@ -2354,7 +2429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2535,6 +2610,13 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>avinash18dce.kumar@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fakeid@gmail.com</t>
         </is>
       </c>
     </row>
@@ -2549,7 +2631,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2728,6 +2810,13 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fakeid@gmail.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>